<commit_message>
ANN regresion ANN classification LR reguarized
</commit_message>
<xml_diff>
--- a/Data from linear regression.xlsx
+++ b/Data from linear regression.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\G531\Documents\8 - Github\ecoli-analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFE6A18F-5B95-4D85-94FF-A6A2C0439204}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C9E26B5A-30B3-42BE-BA66-D6EA9125E434}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3540" yWindow="996" windowWidth="17280" windowHeight="8964" activeTab="1" xr2:uid="{DF8EB005-2047-43EA-86BD-2F95A5983DA9}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t xml:space="preserve">Linear regession without feature selection </t>
   </si>
@@ -41,17 +41,50 @@
     <t>Training error</t>
   </si>
   <si>
-    <t>Test error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">R^2 train </t>
+    <t xml:space="preserve">R^2 Test </t>
+  </si>
+  <si>
+    <t xml:space="preserve">R^2 Train </t>
+  </si>
+  <si>
+    <t>Test Error</t>
+  </si>
+  <si>
+    <t>Regularization linear regression</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Attribute </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Weigth in last fold </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Offset </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mgc </t>
+  </si>
+  <si>
+    <t>gvh</t>
+  </si>
+  <si>
+    <t>lip</t>
+  </si>
+  <si>
+    <t>alm1</t>
+  </si>
+  <si>
+    <t>alm2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="0.0000000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -59,16 +92,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="26">
     <border>
       <left/>
       <right/>
@@ -76,13 +123,437 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="22" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,35 +999,298 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8221CAFF-433C-4CEA-88A6-9B82CAB1737F}">
-  <dimension ref="B5:B8"/>
+  <dimension ref="A3:K22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="Q14" sqref="Q14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="2" max="2" width="12.33203125" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="5" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B5" t="s">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
+      <c r="G3" s="32"/>
+      <c r="H3" s="32"/>
+      <c r="I3" s="32"/>
+      <c r="J3" s="32"/>
+      <c r="K3" s="32"/>
+    </row>
+    <row r="4" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="32"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
+      <c r="G4" s="32"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="32"/>
+      <c r="J4" s="32"/>
+      <c r="K4" s="32"/>
+    </row>
+    <row r="5" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="32"/>
+      <c r="B5" s="18"/>
+      <c r="C5" s="10" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B6" t="s">
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="12"/>
+      <c r="G5" s="14" t="s">
+        <v>5</v>
+      </c>
+      <c r="H5" s="15"/>
+      <c r="I5" s="16"/>
+      <c r="J5" s="32"/>
+      <c r="K5" s="32"/>
+    </row>
+    <row r="6" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="32"/>
+      <c r="B6" s="13" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="7" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B7" t="s">
+      <c r="C6" s="19">
+        <v>0.01</v>
+      </c>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
+      <c r="F6" s="3"/>
+      <c r="G6" s="3">
+        <v>0.01</v>
+      </c>
+      <c r="H6" s="3"/>
+      <c r="I6" s="4"/>
+      <c r="J6" s="32"/>
+      <c r="K6" s="32"/>
+    </row>
+    <row r="7" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="32"/>
+      <c r="B7" s="17" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="5">
+        <v>0.01</v>
+      </c>
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2">
+        <v>0.01</v>
+      </c>
+      <c r="H7" s="2"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="32"/>
+      <c r="K7" s="32"/>
+    </row>
+    <row r="8" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="32"/>
+      <c r="B8" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="C8" s="5">
+        <v>0.1</v>
+      </c>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="2"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="32"/>
+      <c r="K8" s="32"/>
+    </row>
+    <row r="9" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="32"/>
+      <c r="B9" s="13" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="8" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B8" t="s">
-        <v>3</v>
-      </c>
+      <c r="C9" s="7">
+        <v>0.06</v>
+      </c>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8">
+        <v>0.08</v>
+      </c>
+      <c r="H9" s="8"/>
+      <c r="I9" s="9"/>
+      <c r="J9" s="32"/>
+      <c r="K9" s="32"/>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A10" s="32"/>
+      <c r="B10" s="32"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="32"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="32"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
+      <c r="J10" s="32"/>
+      <c r="K10" s="32"/>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A11" s="32"/>
+      <c r="B11" s="32"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="32"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="32"/>
+      <c r="I11" s="32"/>
+      <c r="J11" s="32"/>
+      <c r="K11" s="32"/>
+    </row>
+    <row r="12" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="32"/>
+      <c r="B12" s="32"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="32"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="32"/>
+      <c r="I12" s="32"/>
+      <c r="J12" s="32"/>
+      <c r="K12" s="32"/>
+    </row>
+    <row r="13" spans="1:11" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A13" s="32"/>
+      <c r="B13" s="29" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="30" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13" s="31"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A14" s="32"/>
+      <c r="B14" s="26" t="s">
+        <v>8</v>
+      </c>
+      <c r="C14" s="23">
+        <v>0.50036000000000003</v>
+      </c>
+      <c r="D14" s="20"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="32"/>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A15" s="32"/>
+      <c r="B15" s="27" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="24">
+        <v>1.5896E-2</v>
+      </c>
+      <c r="D15" s="21"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="32"/>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A16" s="32"/>
+      <c r="B16" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="24">
+        <v>3.7335999999999999E-4</v>
+      </c>
+      <c r="D16" s="21"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="32"/>
+      <c r="B17" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="24">
+        <v>4.6464E-4</v>
+      </c>
+      <c r="D17" s="21"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="32"/>
+      <c r="B18" s="27" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="24">
+        <v>1.6808E-2</v>
+      </c>
+      <c r="D18" s="21"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
+    </row>
+    <row r="19" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="32"/>
+      <c r="B19" s="28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" s="25">
+        <v>8.1975999999999993E-3</v>
+      </c>
+      <c r="D19" s="22"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="32"/>
+      <c r="B20" s="32"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="32"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="32"/>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="32"/>
+      <c r="B21" s="32"/>
+      <c r="C21" s="32"/>
+      <c r="D21" s="32"/>
+      <c r="E21" s="32"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="32"/>
     </row>
   </sheetData>
+  <mergeCells count="17">
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:D14"/>
+    <mergeCell ref="C15:D15"/>
+    <mergeCell ref="C16:D16"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="C5:F5"/>
+    <mergeCell ref="C6:F6"/>
+    <mergeCell ref="C7:F7"/>
+    <mergeCell ref="C8:F8"/>
+    <mergeCell ref="C9:F9"/>
+    <mergeCell ref="G6:I6"/>
+    <mergeCell ref="G7:I7"/>
+    <mergeCell ref="G8:I8"/>
+    <mergeCell ref="G9:I9"/>
+    <mergeCell ref="G5:I5"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>